<commit_message>
aggiunti testCase 217-218-219 a seguito fix GWT
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PolisNet\Sanita\fse\it-fse-accreditamento\GATEWAY\A1#111SIS4CAREXX\POLIS-NET_SRL\SIS4CARE\v1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4E84A-E3F0-4AB8-8FEF-A1526BCC582B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B11E9-8A12-4CEE-8884-5F2AE28C77F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="291">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1228,6 +1228,33 @@
   </si>
   <si>
     <t>L'applicativo ripete la chiamata al servizio di validazione ad intervalli regolari finchè non riceve lo status 201 come risposta.</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:24:40Z</t>
+  </si>
+  <si>
+    <t>c67ed7f753b1862b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0fdb7f45a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:31:40Z</t>
+  </si>
+  <si>
+    <t>21e78ef17f69c79c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6464963d8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:33:31Z</t>
+  </si>
+  <si>
+    <t>42ddaacbf188e80a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d1e1dab0e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1321,12 +1348,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1512,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1610,34 +1631,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2116,6 +2109,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED629B79-D92E-7AA4-1663-45E31187106F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3318858A-DC35-C344-F3F4-F2C3A7AA0E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2633,10 +2734,10 @@
   <dimension ref="A1:T580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="J38" sqref="J38:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,14 +2780,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="38"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2704,14 +2805,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -2729,12 +2830,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2753,12 +2854,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -2776,8 +2877,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="1"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -3302,7 +3403,7 @@
       <c r="G18" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="35" t="s">
         <v>231</v>
       </c>
       <c r="I18" s="29" t="s">
@@ -4214,7 +4315,9 @@
       <c r="O37" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="P37" s="30"/>
+      <c r="P37" s="30" t="s">
+        <v>281</v>
+      </c>
       <c r="Q37" s="30"/>
       <c r="R37" s="31"/>
       <c r="S37" s="32"/>
@@ -4222,105 +4325,135 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35">
+    <row r="38" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
         <v>217</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="43" t="s">
+      <c r="F38" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35">
+    <row r="39" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25">
         <v>218</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="43" t="s">
+      <c r="F39" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="J39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="35">
+    <row r="40" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="25">
         <v>219</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="E40" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="43" t="s">
+      <c r="F40" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="I40" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="J40" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="33" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revisionate validation a seguito KO accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PolisNet\Sanita\fse\it-fse-accreditamento\GATEWAY\A1#111SIS4CAREXX\POLIS-NET_SRL\SIS4CARE\v1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B11E9-8A12-4CEE-8884-5F2AE28C77F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33246870-FB94-492B-AF2F-618428F95794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -976,42 +976,6 @@
     <t>POLIS-NET SRL</t>
   </si>
   <si>
-    <t>e1d12748dcc8a3c4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.880c9c99bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-23T16:53:40Z</t>
-  </si>
-  <si>
-    <t>2023-06-26T17:51:40Z</t>
-  </si>
-  <si>
-    <t>eadbe6c86d4a3a7b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.fba176cec5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-27T11:31:10Z</t>
-  </si>
-  <si>
-    <t>cd25a03c2c0c7a19</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.8f04798be6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0e67fa6947a19285</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.84bc5e90d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-27T11:38:22Z</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
@@ -1203,15 +1167,6 @@
     <t>2023-06-27T17:51:40Z</t>
   </si>
   <si>
-    <t>2023-06-27T18:02:29Z</t>
-  </si>
-  <si>
-    <t>4a81f5de48148536</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.48af7c2c0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La riservatezza del documento non viene definita dall'utente e quindi l'errore non può essere riprodotto</t>
   </si>
   <si>
@@ -1255,6 +1210,51 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d1e1dab0e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T10:33:12Z</t>
+  </si>
+  <si>
+    <t>c616ced99760525b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.9142d9255c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T11:04:01Z</t>
+  </si>
+  <si>
+    <t>985c06f953307a52</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.1c0c094857^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>93abf6a4890959e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.c8ff0a3948^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T16:28:50Z</t>
+  </si>
+  <si>
+    <t>2023-07-07T17:36:00Z</t>
+  </si>
+  <si>
+    <t>f0b6469345aac083</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.a5ce9aa251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T17:44:07Z</t>
+  </si>
+  <si>
+    <t>83d331826ef2a2be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.07f77f6030^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2217,6 +2217,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B71FDA-0AB5-ADC3-1521-0BB709234793}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2734,10 +2788,10 @@
   <dimension ref="A1:T580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38:J40"/>
+      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,7 +2911,7 @@
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="40" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D5" s="40"/>
       <c r="F5" s="13"/>
@@ -3012,16 +3066,16 @@
         <v>112</v>
       </c>
       <c r="F10" s="28">
-        <v>45100</v>
+        <v>45114</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>201</v>
+        <v>277</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>202</v>
+        <v>278</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>46</v>
@@ -3056,16 +3110,16 @@
         <v>114</v>
       </c>
       <c r="F11" s="28">
-        <v>45103</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>204</v>
+        <v>45114</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>279</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>46</v>
@@ -3100,16 +3154,16 @@
         <v>116</v>
       </c>
       <c r="F12" s="28">
-        <v>45104</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>207</v>
+        <v>45114</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>284</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>209</v>
+        <v>283</v>
       </c>
       <c r="J12" s="30" t="s">
         <v>46</v>
@@ -3144,16 +3198,16 @@
         <v>118</v>
       </c>
       <c r="F13" s="28">
-        <v>45104</v>
+        <v>45114</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>210</v>
+        <v>286</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>211</v>
+        <v>287</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>46</v>
@@ -3191,13 +3245,13 @@
         <v>45104</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>46</v>
@@ -3210,13 +3264,13 @@
         <v>46</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="O14" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="31"/>
@@ -3245,13 +3299,13 @@
         <v>45104</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J15" s="30" t="s">
         <v>46</v>
@@ -3264,13 +3318,13 @@
         <v>46</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O15" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q15" s="30"/>
       <c r="R15" s="31"/>
@@ -3310,13 +3364,13 @@
         <v>46</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="O16" s="30" t="s">
         <v>47</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="Q16" s="30"/>
       <c r="R16" s="31" t="s">
@@ -3347,13 +3401,13 @@
         <v>45104</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>46</v>
@@ -3366,13 +3420,13 @@
         <v>46</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O17" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P17" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q17" s="30"/>
       <c r="R17" s="31"/>
@@ -3401,13 +3455,13 @@
         <v>45104</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>46</v>
@@ -3420,13 +3474,13 @@
         <v>46</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O18" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P18" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q18" s="30"/>
       <c r="R18" s="31"/>
@@ -3459,7 +3513,7 @@
         <v>47</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
@@ -3497,7 +3551,7 @@
         <v>47</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
@@ -3531,13 +3585,13 @@
         <v>45104</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>46</v>
@@ -3550,13 +3604,13 @@
         <v>46</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O21" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P21" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q21" s="30"/>
       <c r="R21" s="31"/>
@@ -3585,13 +3639,13 @@
         <v>45104</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>46</v>
@@ -3604,13 +3658,13 @@
         <v>46</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O22" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P22" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q22" s="30"/>
       <c r="R22" s="31"/>
@@ -3639,13 +3693,13 @@
         <v>45104</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>46</v>
@@ -3658,13 +3712,13 @@
         <v>46</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O23" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q23" s="30"/>
       <c r="R23" s="31"/>
@@ -3693,13 +3747,13 @@
         <v>45104</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>46</v>
@@ -3712,13 +3766,13 @@
         <v>46</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O24" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q24" s="30"/>
       <c r="R24" s="31"/>
@@ -3747,13 +3801,13 @@
         <v>45104</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="J25" s="30" t="s">
         <v>46</v>
@@ -3766,13 +3820,13 @@
         <v>46</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O25" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q25" s="30"/>
       <c r="R25" s="31"/>
@@ -3801,13 +3855,13 @@
         <v>45104</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>46</v>
@@ -3820,13 +3874,13 @@
         <v>46</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O26" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P26" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q26" s="30"/>
       <c r="R26" s="31"/>
@@ -3855,13 +3909,13 @@
         <v>45104</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>46</v>
@@ -3874,13 +3928,13 @@
         <v>46</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O27" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q27" s="30"/>
       <c r="R27" s="31"/>
@@ -3909,13 +3963,13 @@
         <v>45104</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>46</v>
@@ -3928,13 +3982,13 @@
         <v>46</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O28" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q28" s="30"/>
       <c r="R28" s="31"/>
@@ -3963,13 +4017,13 @@
         <v>45104</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>46</v>
@@ -4143,13 +4197,13 @@
         <v>45104</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>46</v>
@@ -4162,13 +4216,13 @@
         <v>46</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O34" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P34" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q34" s="30"/>
       <c r="R34" s="31"/>
@@ -4197,13 +4251,13 @@
         <v>45104</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>46</v>
@@ -4216,13 +4270,13 @@
         <v>46</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O35" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P35" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q35" s="30"/>
       <c r="R35" s="31"/>
@@ -4251,7 +4305,7 @@
         <v>45104</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
@@ -4259,7 +4313,7 @@
         <v>47</v>
       </c>
       <c r="K36" s="30" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -4293,10 +4347,10 @@
         <v>45104</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="I37" s="29"/>
       <c r="J37" s="30" t="s">
@@ -4310,13 +4364,13 @@
         <v>46</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="O37" s="30" t="s">
         <v>47</v>
       </c>
       <c r="P37" s="30" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="Q37" s="30"/>
       <c r="R37" s="31"/>
@@ -4345,13 +4399,13 @@
         <v>45111</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="H38" s="29" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="J38" s="30" t="s">
         <v>46</v>
@@ -4389,13 +4443,13 @@
         <v>45111</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="I39" s="29" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="J39" s="30" t="s">
         <v>46</v>
@@ -4433,13 +4487,13 @@
         <v>45111</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="H40" s="29" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="J40" s="30" t="s">
         <v>46</v>
@@ -4613,13 +4667,13 @@
         <v>45105</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>46</v>
@@ -4632,13 +4686,13 @@
         <v>46</v>
       </c>
       <c r="N45" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O45" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P45" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q45" s="30"/>
       <c r="R45" s="31"/>
@@ -4667,13 +4721,13 @@
         <v>45105</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J46" s="30" t="s">
         <v>46</v>
@@ -4686,13 +4740,13 @@
         <v>46</v>
       </c>
       <c r="N46" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q46" s="30"/>
       <c r="R46" s="31"/>
@@ -4854,16 +4908,16 @@
         <v>199</v>
       </c>
       <c r="F51" s="28">
-        <v>45104</v>
+        <v>45114</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="J51" s="30" t="s">
         <v>46</v>
@@ -13033,22 +13087,22 @@
         <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="G1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J1" t="s">
         <v>46</v>
@@ -13060,13 +13114,13 @@
         <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="O1" t="s">
         <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="T1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Revert "Update data.json PDF e report-checklist.xlsx"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PolisNet\Sanita\fse\it-fse-accreditamento\GATEWAY\A1#111SIS4CAREXX\POLIS-NET_SRL\SIS4CARE\v1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33246870-FB94-492B-AF2F-618428F95794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4E84A-E3F0-4AB8-8FEF-A1526BCC582B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="282">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -976,6 +976,42 @@
     <t>POLIS-NET SRL</t>
   </si>
   <si>
+    <t>e1d12748dcc8a3c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.880c9c99bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-23T16:53:40Z</t>
+  </si>
+  <si>
+    <t>2023-06-26T17:51:40Z</t>
+  </si>
+  <si>
+    <t>eadbe6c86d4a3a7b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.fba176cec5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-27T11:31:10Z</t>
+  </si>
+  <si>
+    <t>cd25a03c2c0c7a19</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.8f04798be6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0e67fa6947a19285</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.84bc5e90d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-27T11:38:22Z</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
@@ -1167,6 +1203,15 @@
     <t>2023-06-27T17:51:40Z</t>
   </si>
   <si>
+    <t>2023-06-27T18:02:29Z</t>
+  </si>
+  <si>
+    <t>4a81f5de48148536</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.48af7c2c0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>La riservatezza del documento non viene definita dall'utente e quindi l'errore non può essere riprodotto</t>
   </si>
   <si>
@@ -1183,78 +1228,6 @@
   </si>
   <si>
     <t>L'applicativo ripete la chiamata al servizio di validazione ad intervalli regolari finchè non riceve lo status 201 come risposta.</t>
-  </si>
-  <si>
-    <t>2023-07-04T18:24:40Z</t>
-  </si>
-  <si>
-    <t>c67ed7f753b1862b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0fdb7f45a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-04T18:31:40Z</t>
-  </si>
-  <si>
-    <t>21e78ef17f69c79c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6464963d8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-04T18:33:31Z</t>
-  </si>
-  <si>
-    <t>42ddaacbf188e80a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d1e1dab0e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-07T10:33:12Z</t>
-  </si>
-  <si>
-    <t>c616ced99760525b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.9142d9255c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-07T11:04:01Z</t>
-  </si>
-  <si>
-    <t>985c06f953307a52</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.1c0c094857^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>93abf6a4890959e1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.c8ff0a3948^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-07T16:28:50Z</t>
-  </si>
-  <si>
-    <t>2023-07-07T17:36:00Z</t>
-  </si>
-  <si>
-    <t>f0b6469345aac083</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.a5ce9aa251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-07T17:44:07Z</t>
-  </si>
-  <si>
-    <t>83d331826ef2a2be</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.07f77f6030^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1348,6 +1321,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1533,7 +1512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1631,6 +1610,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2109,168 +2116,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>466725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED629B79-D92E-7AA4-1663-45E31187106F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10687050" cy="23917275"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>466725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3318858A-DC35-C344-F3F4-F2C3A7AA0E37}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10687050" cy="23917275"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>466725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B71FDA-0AB5-ADC3-1521-0BB709234793}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10687050" cy="23917275"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2788,10 +2633,10 @@
   <dimension ref="A1:T580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,14 +2679,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2859,14 +2704,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -2884,12 +2729,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="3"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2908,12 +2753,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="40"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="50"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -2931,8 +2776,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="1"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -3066,16 +2911,16 @@
         <v>112</v>
       </c>
       <c r="F10" s="28">
-        <v>45114</v>
+        <v>45100</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>276</v>
+        <v>203</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>46</v>
@@ -3110,16 +2955,16 @@
         <v>114</v>
       </c>
       <c r="F11" s="28">
-        <v>45114</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>279</v>
+        <v>45103</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>204</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>280</v>
+        <v>205</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>281</v>
+        <v>206</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>46</v>
@@ -3154,16 +2999,16 @@
         <v>116</v>
       </c>
       <c r="F12" s="28">
-        <v>45114</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>284</v>
+        <v>45104</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>207</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>282</v>
+        <v>208</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
       <c r="J12" s="30" t="s">
         <v>46</v>
@@ -3198,16 +3043,16 @@
         <v>118</v>
       </c>
       <c r="F13" s="28">
-        <v>45114</v>
+        <v>45104</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>285</v>
+        <v>212</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>286</v>
+        <v>210</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>46</v>
@@ -3245,13 +3090,13 @@
         <v>45104</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>46</v>
@@ -3264,13 +3109,13 @@
         <v>46</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="O14" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="31"/>
@@ -3299,13 +3144,13 @@
         <v>45104</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="J15" s="30" t="s">
         <v>46</v>
@@ -3318,13 +3163,13 @@
         <v>46</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O15" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q15" s="30"/>
       <c r="R15" s="31"/>
@@ -3364,13 +3209,13 @@
         <v>46</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="O16" s="30" t="s">
         <v>47</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="Q16" s="30"/>
       <c r="R16" s="31" t="s">
@@ -3401,13 +3246,13 @@
         <v>45104</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>46</v>
@@ -3420,13 +3265,13 @@
         <v>46</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O17" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P17" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q17" s="30"/>
       <c r="R17" s="31"/>
@@ -3455,13 +3300,13 @@
         <v>45104</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>219</v>
+        <v>228</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>231</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>46</v>
@@ -3474,13 +3319,13 @@
         <v>46</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O18" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P18" s="30" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="Q18" s="30"/>
       <c r="R18" s="31"/>
@@ -3513,7 +3358,7 @@
         <v>47</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
@@ -3551,7 +3396,7 @@
         <v>47</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
@@ -3585,13 +3430,13 @@
         <v>45104</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>46</v>
@@ -3604,13 +3449,13 @@
         <v>46</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O21" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P21" s="30" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="Q21" s="30"/>
       <c r="R21" s="31"/>
@@ -3639,13 +3484,13 @@
         <v>45104</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>46</v>
@@ -3658,13 +3503,13 @@
         <v>46</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O22" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P22" s="30" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="Q22" s="30"/>
       <c r="R22" s="31"/>
@@ -3693,13 +3538,13 @@
         <v>45104</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>46</v>
@@ -3712,13 +3557,13 @@
         <v>46</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O23" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q23" s="30"/>
       <c r="R23" s="31"/>
@@ -3747,13 +3592,13 @@
         <v>45104</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>46</v>
@@ -3766,13 +3611,13 @@
         <v>46</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O24" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q24" s="30"/>
       <c r="R24" s="31"/>
@@ -3801,13 +3646,13 @@
         <v>45104</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="J25" s="30" t="s">
         <v>46</v>
@@ -3820,13 +3665,13 @@
         <v>46</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O25" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q25" s="30"/>
       <c r="R25" s="31"/>
@@ -3855,13 +3700,13 @@
         <v>45104</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>46</v>
@@ -3874,13 +3719,13 @@
         <v>46</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O26" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P26" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q26" s="30"/>
       <c r="R26" s="31"/>
@@ -3909,13 +3754,13 @@
         <v>45104</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>46</v>
@@ -3928,13 +3773,13 @@
         <v>46</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O27" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q27" s="30"/>
       <c r="R27" s="31"/>
@@ -3963,13 +3808,13 @@
         <v>45104</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>46</v>
@@ -3982,13 +3827,13 @@
         <v>46</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O28" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="Q28" s="30"/>
       <c r="R28" s="31"/>
@@ -4017,13 +3862,13 @@
         <v>45104</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>46</v>
@@ -4197,13 +4042,13 @@
         <v>45104</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>46</v>
@@ -4216,13 +4061,13 @@
         <v>46</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="O34" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P34" s="30" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="Q34" s="30"/>
       <c r="R34" s="31"/>
@@ -4251,13 +4096,13 @@
         <v>45104</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>46</v>
@@ -4270,13 +4115,13 @@
         <v>46</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="O35" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P35" s="30" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="Q35" s="30"/>
       <c r="R35" s="31"/>
@@ -4305,7 +4150,7 @@
         <v>45104</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
@@ -4313,7 +4158,7 @@
         <v>47</v>
       </c>
       <c r="K36" s="30" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -4347,10 +4192,10 @@
         <v>45104</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="I37" s="29"/>
       <c r="J37" s="30" t="s">
@@ -4364,14 +4209,12 @@
         <v>46</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="O37" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="P37" s="30" t="s">
-        <v>266</v>
-      </c>
+      <c r="P37" s="30"/>
       <c r="Q37" s="30"/>
       <c r="R37" s="31"/>
       <c r="S37" s="32"/>
@@ -4379,135 +4222,105 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25">
+    <row r="38" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="35">
         <v>217</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="28">
-        <v>45111</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="I38" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="J38" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="33" t="s">
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25">
+    <row r="39" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="35">
         <v>218</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="F39" s="28">
-        <v>45111</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="I39" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="J39" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="31"/>
-      <c r="S39" s="32"/>
-      <c r="T39" s="33" t="s">
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="40"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="25">
+    <row r="40" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="35">
         <v>219</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="F40" s="28">
-        <v>45111</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="I40" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="J40" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="31"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="33" t="s">
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="40"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="43" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4667,13 +4480,13 @@
         <v>45105</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>46</v>
@@ -4686,13 +4499,13 @@
         <v>46</v>
       </c>
       <c r="N45" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="O45" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P45" s="30" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="Q45" s="30"/>
       <c r="R45" s="31"/>
@@ -4721,13 +4534,13 @@
         <v>45105</v>
       </c>
       <c r="G46" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="I46" s="29" t="s">
         <v>264</v>
-      </c>
-      <c r="H46" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="I46" s="29" t="s">
-        <v>252</v>
       </c>
       <c r="J46" s="30" t="s">
         <v>46</v>
@@ -4740,13 +4553,13 @@
         <v>46</v>
       </c>
       <c r="N46" s="30" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="Q46" s="30"/>
       <c r="R46" s="31"/>
@@ -4908,16 +4721,16 @@
         <v>199</v>
       </c>
       <c r="F51" s="28">
-        <v>45114</v>
+        <v>45104</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="J51" s="30" t="s">
         <v>46</v>
@@ -13087,22 +12900,22 @@
         <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="F1" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="I1" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="J1" t="s">
         <v>46</v>
@@ -13114,13 +12927,13 @@
         <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="O1" t="s">
         <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="T1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Revert "Revert "Update data.json PDF e report-checklist.xlsx""
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PolisNet\Sanita\fse\it-fse-accreditamento\GATEWAY\A1#111SIS4CAREXX\POLIS-NET_SRL\SIS4CARE\v1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4E84A-E3F0-4AB8-8FEF-A1526BCC582B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33246870-FB94-492B-AF2F-618428F95794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="291">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -976,42 +976,6 @@
     <t>POLIS-NET SRL</t>
   </si>
   <si>
-    <t>e1d12748dcc8a3c4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.880c9c99bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-23T16:53:40Z</t>
-  </si>
-  <si>
-    <t>2023-06-26T17:51:40Z</t>
-  </si>
-  <si>
-    <t>eadbe6c86d4a3a7b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.fba176cec5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-27T11:31:10Z</t>
-  </si>
-  <si>
-    <t>cd25a03c2c0c7a19</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.8f04798be6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0e67fa6947a19285</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.84bc5e90d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-27T11:38:22Z</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
@@ -1203,15 +1167,6 @@
     <t>2023-06-27T17:51:40Z</t>
   </si>
   <si>
-    <t>2023-06-27T18:02:29Z</t>
-  </si>
-  <si>
-    <t>4a81f5de48148536</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.48af7c2c0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La riservatezza del documento non viene definita dall'utente e quindi l'errore non può essere riprodotto</t>
   </si>
   <si>
@@ -1228,6 +1183,78 @@
   </si>
   <si>
     <t>L'applicativo ripete la chiamata al servizio di validazione ad intervalli regolari finchè non riceve lo status 201 come risposta.</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:24:40Z</t>
+  </si>
+  <si>
+    <t>c67ed7f753b1862b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0fdb7f45a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:31:40Z</t>
+  </si>
+  <si>
+    <t>21e78ef17f69c79c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6464963d8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-04T18:33:31Z</t>
+  </si>
+  <si>
+    <t>42ddaacbf188e80a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.d1e1dab0e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T10:33:12Z</t>
+  </si>
+  <si>
+    <t>c616ced99760525b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.9142d9255c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T11:04:01Z</t>
+  </si>
+  <si>
+    <t>985c06f953307a52</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.1c0c094857^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>93abf6a4890959e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.c8ff0a3948^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T16:28:50Z</t>
+  </si>
+  <si>
+    <t>2023-07-07T17:36:00Z</t>
+  </si>
+  <si>
+    <t>f0b6469345aac083</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.a5ce9aa251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-07-07T17:44:07Z</t>
+  </si>
+  <si>
+    <t>83d331826ef2a2be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.a4e181d744702b6d7d921597e1fb886122e5313dca0d2d59233ab406f4ccd39e.07f77f6030^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1321,12 +1348,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1512,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1610,34 +1631,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2116,6 +2109,168 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED629B79-D92E-7AA4-1663-45E31187106F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3318858A-DC35-C344-F3F4-F2C3A7AA0E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B71FDA-0AB5-ADC3-1521-0BB709234793}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10687050" cy="23917275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2633,10 +2788,10 @@
   <dimension ref="A1:T580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,14 +2834,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="38"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2704,14 +2859,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -2729,12 +2884,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2753,12 +2908,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" s="50"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="40"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -2776,8 +2931,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="1"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2911,16 +3066,16 @@
         <v>112</v>
       </c>
       <c r="F10" s="28">
-        <v>45100</v>
+        <v>45114</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>201</v>
+        <v>277</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>202</v>
+        <v>278</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>46</v>
@@ -2955,16 +3110,16 @@
         <v>114</v>
       </c>
       <c r="F11" s="28">
-        <v>45103</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>204</v>
+        <v>45114</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>279</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>46</v>
@@ -2999,16 +3154,16 @@
         <v>116</v>
       </c>
       <c r="F12" s="28">
-        <v>45104</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>207</v>
+        <v>45114</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>284</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>209</v>
+        <v>283</v>
       </c>
       <c r="J12" s="30" t="s">
         <v>46</v>
@@ -3043,16 +3198,16 @@
         <v>118</v>
       </c>
       <c r="F13" s="28">
-        <v>45104</v>
+        <v>45114</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>210</v>
+        <v>286</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>211</v>
+        <v>287</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>46</v>
@@ -3090,13 +3245,13 @@
         <v>45104</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>46</v>
@@ -3109,13 +3264,13 @@
         <v>46</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="O14" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="31"/>
@@ -3144,13 +3299,13 @@
         <v>45104</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J15" s="30" t="s">
         <v>46</v>
@@ -3163,13 +3318,13 @@
         <v>46</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O15" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q15" s="30"/>
       <c r="R15" s="31"/>
@@ -3209,13 +3364,13 @@
         <v>46</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="O16" s="30" t="s">
         <v>47</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="Q16" s="30"/>
       <c r="R16" s="31" t="s">
@@ -3246,13 +3401,13 @@
         <v>45104</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>46</v>
@@ -3265,13 +3420,13 @@
         <v>46</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O17" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P17" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q17" s="30"/>
       <c r="R17" s="31"/>
@@ -3300,13 +3455,13 @@
         <v>45104</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="H18" s="45" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>219</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>46</v>
@@ -3319,13 +3474,13 @@
         <v>46</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O18" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P18" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q18" s="30"/>
       <c r="R18" s="31"/>
@@ -3358,7 +3513,7 @@
         <v>47</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
@@ -3396,7 +3551,7 @@
         <v>47</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
@@ -3430,13 +3585,13 @@
         <v>45104</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>46</v>
@@ -3449,13 +3604,13 @@
         <v>46</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O21" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P21" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q21" s="30"/>
       <c r="R21" s="31"/>
@@ -3484,13 +3639,13 @@
         <v>45104</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>46</v>
@@ -3503,13 +3658,13 @@
         <v>46</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O22" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P22" s="30" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="Q22" s="30"/>
       <c r="R22" s="31"/>
@@ -3538,13 +3693,13 @@
         <v>45104</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>46</v>
@@ -3557,13 +3712,13 @@
         <v>46</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O23" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q23" s="30"/>
       <c r="R23" s="31"/>
@@ -3592,13 +3747,13 @@
         <v>45104</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>46</v>
@@ -3611,13 +3766,13 @@
         <v>46</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O24" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q24" s="30"/>
       <c r="R24" s="31"/>
@@ -3646,13 +3801,13 @@
         <v>45104</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="J25" s="30" t="s">
         <v>46</v>
@@ -3665,13 +3820,13 @@
         <v>46</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O25" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q25" s="30"/>
       <c r="R25" s="31"/>
@@ -3700,13 +3855,13 @@
         <v>45104</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>46</v>
@@ -3719,13 +3874,13 @@
         <v>46</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O26" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P26" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q26" s="30"/>
       <c r="R26" s="31"/>
@@ -3754,13 +3909,13 @@
         <v>45104</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>46</v>
@@ -3773,13 +3928,13 @@
         <v>46</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O27" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P27" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q27" s="30"/>
       <c r="R27" s="31"/>
@@ -3808,13 +3963,13 @@
         <v>45104</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>46</v>
@@ -3827,13 +3982,13 @@
         <v>46</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O28" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="Q28" s="30"/>
       <c r="R28" s="31"/>
@@ -3862,13 +4017,13 @@
         <v>45104</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>46</v>
@@ -4042,13 +4197,13 @@
         <v>45104</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>46</v>
@@ -4061,13 +4216,13 @@
         <v>46</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O34" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P34" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q34" s="30"/>
       <c r="R34" s="31"/>
@@ -4096,13 +4251,13 @@
         <v>45104</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>46</v>
@@ -4115,13 +4270,13 @@
         <v>46</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O35" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P35" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q35" s="30"/>
       <c r="R35" s="31"/>
@@ -4150,7 +4305,7 @@
         <v>45104</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
@@ -4158,7 +4313,7 @@
         <v>47</v>
       </c>
       <c r="K36" s="30" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -4192,10 +4347,10 @@
         <v>45104</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="I37" s="29"/>
       <c r="J37" s="30" t="s">
@@ -4209,12 +4364,14 @@
         <v>46</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="O37" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="P37" s="30"/>
+      <c r="P37" s="30" t="s">
+        <v>266</v>
+      </c>
       <c r="Q37" s="30"/>
       <c r="R37" s="31"/>
       <c r="S37" s="32"/>
@@ -4222,105 +4379,135 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35">
+    <row r="38" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
         <v>217</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="43" t="s">
+      <c r="F38" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35">
+    <row r="39" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25">
         <v>218</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="43" t="s">
+      <c r="F39" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="J39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="44" customFormat="1" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="35">
+    <row r="40" spans="1:20" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="25">
         <v>219</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="E40" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="43" t="s">
+      <c r="F40" s="28">
+        <v>45111</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="I40" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="33" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4480,13 +4667,13 @@
         <v>45105</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>46</v>
@@ -4499,13 +4686,13 @@
         <v>46</v>
       </c>
       <c r="N45" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O45" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P45" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q45" s="30"/>
       <c r="R45" s="31"/>
@@ -4534,13 +4721,13 @@
         <v>45105</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J46" s="30" t="s">
         <v>46</v>
@@ -4553,13 +4740,13 @@
         <v>46</v>
       </c>
       <c r="N46" s="30" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>46</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="Q46" s="30"/>
       <c r="R46" s="31"/>
@@ -4721,16 +4908,16 @@
         <v>199</v>
       </c>
       <c r="F51" s="28">
-        <v>45104</v>
+        <v>45114</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="J51" s="30" t="s">
         <v>46</v>
@@ -12900,22 +13087,22 @@
         <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="G1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="J1" t="s">
         <v>46</v>
@@ -12927,13 +13114,13 @@
         <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="O1" t="s">
         <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="T1" t="s">
         <v>49</v>

</xml_diff>